<commit_message>
added some notes for buzzard coulee, vinales and saricicek (last events i still needed to do preliminary analysis on)
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/usg-ground-based-comparison_EDITED.xlsx
+++ b/speed_radiant_difference/usg-ground-based-comparison_EDITED.xlsx
@@ -1132,12 +1132,12 @@
   <dimension ref="A1:AL40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AF18" activeCellId="0" sqref="AF18"/>
+      <selection pane="bottomLeft" activeCell="AH13" activeCellId="0" sqref="AH13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.57"/>

</xml_diff>

<commit_message>
went through a bunch of events with peter and made notes in the excel file for later -- need to compute lengths for a bunch of these events using the lightcurve/glm analysis talked about
</commit_message>
<xml_diff>
--- a/speed_radiant_difference/usg-ground-based-comparison_EDITED.xlsx
+++ b/speed_radiant_difference/usg-ground-based-comparison_EDITED.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t xml:space="preserve">Borovicka et al. 2013. The Kosice meteorite fall: Atmospheric trajectory, fragmentation, and orbit, Meteoritics and Planetary Science, 48, 1757-1779.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check begin height w/ lightcurve analysis</t>
   </si>
   <si>
     <t xml:space="preserve">Motopi Pan </t>
@@ -343,6 +346,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">recompute length using lightcurve as well</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flensburg</t>
   </si>
   <si>
@@ -478,10 +484,16 @@
     <t xml:space="preserve">https://ssd.jpl.nasa.gov/tools/sbdb_lookup.html#/?sstr=54254967</t>
   </si>
   <si>
+    <t xml:space="preserve">nothing</t>
+  </si>
+  <si>
     <t xml:space="preserve">2019MO</t>
   </si>
   <si>
     <t xml:space="preserve">https://ssd.jpl.nasa.gov/tools/sbdb_lookup.html#/?sstr=3842925&amp;view=OPC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLM </t>
   </si>
   <si>
     <t xml:space="preserve">Ozerski</t>
@@ -518,6 +530,9 @@
       </rPr>
       <t xml:space="preserve"> 193:105034. https://doi.org/10.1016/j.pss.2020.105034.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">lightcurve (same thing as 2019MO)</t>
   </si>
   <si>
     <t xml:space="preserve">USG values</t>
@@ -1134,7 +1149,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AH13" activeCellId="0" sqref="AH13"/>
+      <selection pane="bottomLeft" activeCell="AJ20" activeCellId="0" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2118,10 +2133,13 @@
       <c r="AH11" s="0" t="n">
         <v>17.4</v>
       </c>
+      <c r="AI11" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="19" t="n">
         <v>95.19</v>
@@ -2176,10 +2194,10 @@
       <c r="AC12" s="33"/>
       <c r="AD12" s="31"/>
       <c r="AE12" s="36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AL12" s="37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,15 +2268,15 @@
         <v>124.8</v>
       </c>
       <c r="AG13" s="0" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="AH13" s="0" t="n">
-        <v>27.8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="19" t="n">
         <v>177.566</v>
@@ -2314,7 +2332,7 @@
       <c r="AD14" s="31"/>
       <c r="AE14" s="31"/>
       <c r="AL14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,7 +2411,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16" s="19" t="n">
         <v>6.74</v>
@@ -2449,7 +2467,7 @@
       <c r="AD16" s="31"/>
       <c r="AE16" s="31"/>
       <c r="AL16" s="37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2543,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" s="19" t="n">
         <v>346.41</v>
@@ -2581,7 +2599,7 @@
       <c r="AD18" s="31"/>
       <c r="AE18" s="31"/>
       <c r="AL18" s="37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2657,7 +2675,7 @@
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="19" t="n">
         <v>232.2</v>
@@ -2713,7 +2731,7 @@
       <c r="AD20" s="31"/>
       <c r="AE20" s="31"/>
       <c r="AL20" s="37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,10 +2806,13 @@
       <c r="AH21" s="0" t="n">
         <v>38.69</v>
       </c>
+      <c r="AI21" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B22" s="19" t="n">
         <v>188.1</v>
@@ -2846,10 +2867,10 @@
       <c r="AC22" s="33"/>
       <c r="AD22" s="31"/>
       <c r="AE22" s="36" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AL22" s="37" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,7 +2949,7 @@
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B24" s="19" t="n">
         <v>156.5</v>
@@ -2983,10 +3004,10 @@
       <c r="AC24" s="33"/>
       <c r="AD24" s="31"/>
       <c r="AE24" s="36" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="AL24" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,7 +3083,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B26" s="19" t="n">
         <v>319.6</v>
@@ -3117,10 +3138,10 @@
       <c r="AC26" s="33"/>
       <c r="AD26" s="31"/>
       <c r="AE26" s="36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AL26" s="37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,7 +3220,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B28" s="19" t="n">
         <v>171.8</v>
@@ -3254,10 +3275,10 @@
       <c r="AC28" s="33"/>
       <c r="AD28" s="31"/>
       <c r="AE28" s="36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AL28" s="37" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,10 +3345,16 @@
       </c>
       <c r="AD29" s="26"/>
       <c r="AE29" s="26"/>
+      <c r="AG29" s="0" t="n">
+        <v>72.24</v>
+      </c>
+      <c r="AH29" s="0" t="n">
+        <v>23.313</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B30" s="19" t="n">
         <v>243.6</v>
@@ -3381,7 +3408,7 @@
       <c r="AD30" s="31"/>
       <c r="AE30" s="36"/>
       <c r="AL30" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,7 +3479,7 @@
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B32" s="19" t="n">
         <v>129.3</v>
@@ -3506,7 +3533,7 @@
       <c r="AD32" s="31"/>
       <c r="AE32" s="36"/>
       <c r="AL32" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3569,10 +3596,13 @@
       <c r="AC33" s="30"/>
       <c r="AD33" s="26"/>
       <c r="AE33" s="26"/>
+      <c r="AI33" s="0" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B34" s="19" t="n">
         <v>109.7</v>
@@ -3626,7 +3656,7 @@
       <c r="AD34" s="31"/>
       <c r="AE34" s="36"/>
       <c r="AL34" s="41" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3681,10 +3711,13 @@
       <c r="AC35" s="30"/>
       <c r="AD35" s="26"/>
       <c r="AE35" s="26"/>
+      <c r="AI35" s="0" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="42" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B36" s="43" t="n">
         <v>238</v>
@@ -3739,10 +3772,10 @@
       <c r="AC36" s="45"/>
       <c r="AD36" s="43"/>
       <c r="AE36" s="43" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AL36" s="37" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,17 +3833,20 @@
       </c>
       <c r="AD37" s="46"/>
       <c r="AE37" s="46"/>
+      <c r="AI37" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="39"/>
       <c r="D39" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="49"/>
       <c r="D40" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>